<commit_message>
Refinamiento de los requerimientos y su priorización.
</commit_message>
<xml_diff>
--- a/Requerimientos/Backlog_producto.xlsx
+++ b/Requerimientos/Backlog_producto.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="FEATURES" sheetId="1" r:id="rId1"/>
+    <sheet name="ESCENARIOS_NEGOCIO" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FEATURES!$A$3:$J$90</definedName>
+    <definedName name="ESCENARIOS_NEGOCIO">ESCENARIOS_NEGOCIO!$B$3:$E$19</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="226">
   <si>
     <t>BACKLOG DEL PRODUCTO</t>
   </si>
@@ -638,13 +643,76 @@
   </si>
   <si>
     <t>CA-006.05.01</t>
+  </si>
+  <si>
+    <t>US-007.01</t>
+  </si>
+  <si>
+    <t>RELEASE</t>
+  </si>
+  <si>
+    <t>SPRINT</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>TITULO</t>
+  </si>
+  <si>
+    <t>EN001</t>
+  </si>
+  <si>
+    <t>Ejecución de una tarea de negocio</t>
+  </si>
+  <si>
+    <t>PRIORIDAD</t>
+  </si>
+  <si>
+    <t>MUY ALTA</t>
+  </si>
+  <si>
+    <t>ESCENARIO</t>
+  </si>
+  <si>
+    <t>ID_ESCENARIO</t>
+  </si>
+  <si>
+    <t>1. Un usuario ingresa al Worklist y se presenta toda la lista de tareas (instancias) que pertenecen a los grupos de usuarios asignados al participante y las asignadas al usuario.
+2. El usuario selecciona una tarea asignada a él para iniciar el trabajo. 
+3. El usuario registra comentarios a la tarea.
+4. Una vez ejecutada la tarea el usuario completa el trabajo y la instancia de la tarea finaliza.</t>
+  </si>
+  <si>
+    <t>EN002</t>
+  </si>
+  <si>
+    <t>EN003</t>
+  </si>
+  <si>
+    <t>Registro de Definiciones de Tarea</t>
+  </si>
+  <si>
+    <t>1. El administrador realiza el registro de una definición de una nueva tarea.
+2. La tarea queda disponible para ser instanciada por el usuario perteneciente a el o los participantes designados de la tarea.</t>
+  </si>
+  <si>
+    <t>1. Un usuario ingresa al Worklist y se presenta toda la lista de tareas (instancias) que pertenecen a los grupos de usuarios asignados al participante y las asignadas al usuario.
+2. El usuario no puede iniciar tareas no asignadas a él.
+3. El usuario debe asignarse una tarea para poder iniciar la ejecución de la tarea.</t>
+  </si>
+  <si>
+    <t>Visualización de tareas del usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,8 +742,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -718,8 +802,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -727,11 +823,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -756,6 +867,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,382 +944,382 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="D3" t="str">
+          <cell r="E3" t="str">
             <v>Añadir adjuntos</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="D4" t="str">
+          <cell r="E4" t="str">
             <v>Añadir comentario</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="D5" t="str">
+          <cell r="E5" t="str">
             <v>Reclamar la tarea</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="D6" t="str">
+          <cell r="E6" t="str">
             <v>Realizar reclamo de tarea en lote</v>
           </cell>
         </row>
         <row r="7">
-          <cell r="D7" t="str">
+          <cell r="E7" t="str">
             <v>Marcar tarea completada</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="D8" t="str">
+          <cell r="E8" t="str">
             <v>Marcar tarea completada en lote</v>
           </cell>
         </row>
         <row r="9">
-          <cell r="D9" t="str">
+          <cell r="E9" t="str">
             <v>Delegar la tarea</v>
           </cell>
         </row>
         <row r="10">
-          <cell r="D10" t="str">
+          <cell r="E10" t="str">
             <v>Delegar la tarea en lote</v>
           </cell>
         </row>
         <row r="11">
-          <cell r="D11" t="str">
+          <cell r="E11" t="str">
             <v>Eliminar adjunto</v>
           </cell>
         </row>
         <row r="12">
-          <cell r="D12" t="str">
+          <cell r="E12" t="str">
             <v>Eliminar comentario</v>
           </cell>
         </row>
         <row r="13">
-          <cell r="D13" t="str">
+          <cell r="E13" t="str">
             <v>Eliminar falla</v>
           </cell>
         </row>
         <row r="14">
-          <cell r="D14" t="str">
+          <cell r="E14" t="str">
             <v>Eliminar salida de la tarea</v>
           </cell>
         </row>
         <row r="15">
-          <cell r="D15" t="str">
+          <cell r="E15" t="str">
             <v>Fallar la tarea</v>
           </cell>
         </row>
         <row r="16">
-          <cell r="D16" t="str">
+          <cell r="E16" t="str">
             <v>Fallar tareas en lote</v>
           </cell>
         </row>
         <row r="17">
-          <cell r="D17" t="str">
+          <cell r="E17" t="str">
             <v>Mover tarea adelante</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="D18" t="str">
+          <cell r="E18" t="str">
             <v>Mover tarea adelante en lote</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="D19" t="str">
+          <cell r="E19" t="str">
             <v>Obtener adjunto</v>
           </cell>
         </row>
         <row r="20">
-          <cell r="D20" t="str">
+          <cell r="E20" t="str">
             <v>Obtener información de adjuntos</v>
           </cell>
         </row>
         <row r="21">
-          <cell r="D21" t="str">
+          <cell r="E21" t="str">
             <v>Obtener comentarios</v>
           </cell>
         </row>
         <row r="22">
-          <cell r="D22" t="str">
+          <cell r="E22" t="str">
             <v>Obtener falla de tarea</v>
           </cell>
         </row>
         <row r="23">
-          <cell r="D23" t="str">
+          <cell r="E23" t="str">
             <v>Obtener información de entrada a la tarea</v>
           </cell>
         </row>
         <row r="24">
-          <cell r="D24" t="str">
+          <cell r="E24" t="str">
             <v>Obtener resultado de accion de finalización de la tarea</v>
           </cell>
         </row>
         <row r="25">
-          <cell r="D25" t="str">
+          <cell r="E25" t="str">
             <v>Obtener salida de la tarea</v>
           </cell>
         </row>
         <row r="26">
-          <cell r="D26" t="str">
+          <cell r="E26" t="str">
             <v>Obtener la tarea padre</v>
           </cell>
         </row>
         <row r="27">
-          <cell r="D27" t="str">
+          <cell r="E27" t="str">
             <v>Obtener Identificador de la tarea padre</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="D28" t="str">
+          <cell r="E28" t="str">
             <v>Obtener visualización de la tarea</v>
           </cell>
         </row>
         <row r="29">
-          <cell r="D29" t="str">
+          <cell r="E29" t="str">
             <v>Obtener tipos de visualizaciones</v>
           </cell>
         </row>
         <row r="30">
-          <cell r="D30" t="str">
+          <cell r="E30" t="str">
             <v>Obtener identificadores de la tarea</v>
           </cell>
         </row>
         <row r="31">
-          <cell r="D31" t="str">
+          <cell r="E31" t="str">
             <v>Obtener Subtareas</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="D32" t="str">
+          <cell r="E32" t="str">
             <v>Obtener Descripcion de la tarea</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="D33" t="str">
+          <cell r="E33" t="str">
             <v>Obtener detalles de la tarea</v>
           </cell>
         </row>
         <row r="34">
-          <cell r="D34" t="str">
+          <cell r="E34" t="str">
             <v>Obtener historia de la tarea</v>
           </cell>
         </row>
         <row r="35">
-          <cell r="D35" t="str">
+          <cell r="E35" t="str">
             <v>Obteher Datos de Instancia de la Tarea</v>
           </cell>
         </row>
         <row r="36">
-          <cell r="D36" t="str">
+          <cell r="E36" t="str">
             <v>Obtener las operaciones de la tarea</v>
           </cell>
         </row>
         <row r="37">
-          <cell r="D37" t="str">
+          <cell r="E37" t="str">
             <v>Determinar si tiene subtareas</v>
           </cell>
         </row>
         <row r="38">
-          <cell r="D38" t="str">
+          <cell r="E38" t="str">
             <v>Instanciar subtarea</v>
           </cell>
         </row>
         <row r="39">
-          <cell r="D39" t="str">
+          <cell r="E39" t="str">
             <v>Determinar si es una subtarea</v>
           </cell>
         </row>
         <row r="40">
-          <cell r="D40" t="str">
+          <cell r="E40" t="str">
             <v>Liberar la tarea</v>
           </cell>
         </row>
         <row r="41">
-          <cell r="D41" t="str">
+          <cell r="E41" t="str">
             <v>Liberar tareas en lote</v>
           </cell>
         </row>
         <row r="42">
-          <cell r="D42" t="str">
+          <cell r="E42" t="str">
             <v>Remover tarea</v>
           </cell>
         </row>
         <row r="43">
-          <cell r="D43" t="str">
-            <v>Remiver tarea en lote</v>
+          <cell r="E43" t="str">
+            <v>Remover tarea en lote</v>
           </cell>
         </row>
         <row r="44">
-          <cell r="D44" t="str">
+          <cell r="E44" t="str">
             <v>Re-iniciar la tarea</v>
           </cell>
         </row>
         <row r="45">
-          <cell r="D45" t="str">
+          <cell r="E45" t="str">
             <v>Re-iniciar tareas en lote</v>
           </cell>
         </row>
         <row r="46">
-          <cell r="D46" t="str">
+          <cell r="E46" t="str">
             <v>Establecer falla de la tarea</v>
           </cell>
         </row>
         <row r="47">
-          <cell r="D47" t="str">
+          <cell r="E47" t="str">
             <v>Establecer la salida de la tarea</v>
           </cell>
         </row>
         <row r="48">
-          <cell r="D48" t="str">
+          <cell r="E48" t="str">
             <v>Establecer la prioridad</v>
           </cell>
         </row>
         <row r="49">
-          <cell r="D49" t="str">
+          <cell r="E49" t="str">
             <v>Establecer prioridad en lote</v>
           </cell>
         </row>
         <row r="50">
-          <cell r="D50" t="str">
+          <cell r="E50" t="str">
             <v>Establecer Expresion de fecha limite de completamiento</v>
           </cell>
         </row>
         <row r="51">
-          <cell r="D51" t="str">
+          <cell r="E51" t="str">
             <v>Establecer Expresion de fecha limite de duracion</v>
           </cell>
         </row>
         <row r="52">
-          <cell r="D52" t="str">
+          <cell r="E52" t="str">
             <v>Establecer Expresión de fecha limite para inicio de tarea</v>
           </cell>
         </row>
         <row r="53">
-          <cell r="D53" t="str">
+          <cell r="E53" t="str">
             <v>Establecer expresion de duración de inicio de tarea</v>
           </cell>
         </row>
         <row r="54">
-          <cell r="D54" t="str">
+          <cell r="E54" t="str">
             <v>Saltar la tarea</v>
           </cell>
         </row>
         <row r="55">
-          <cell r="D55" t="str">
+          <cell r="E55" t="str">
             <v>Saltar tareas en lote</v>
           </cell>
         </row>
         <row r="56">
-          <cell r="D56" t="str">
+          <cell r="E56" t="str">
             <v>Iniciar la tarea</v>
           </cell>
         </row>
         <row r="57">
-          <cell r="D57" t="str">
+          <cell r="E57" t="str">
             <v>Iniciar tareas en lote</v>
           </cell>
         </row>
         <row r="58">
-          <cell r="D58" t="str">
+          <cell r="E58" t="str">
             <v>Detener tarea</v>
           </cell>
         </row>
         <row r="59">
-          <cell r="D59" t="str">
+          <cell r="E59" t="str">
             <v>Detener tareas en lote</v>
           </cell>
         </row>
         <row r="60">
-          <cell r="D60" t="str">
+          <cell r="E60" t="str">
             <v>Suspender la tarea</v>
           </cell>
         </row>
         <row r="61">
-          <cell r="D61" t="str">
+          <cell r="E61" t="str">
             <v>Suspender tareas en lote</v>
           </cell>
         </row>
         <row r="62">
-          <cell r="D62" t="str">
+          <cell r="E62" t="str">
             <v>Suspender tarea hasta condicion</v>
           </cell>
         </row>
         <row r="63">
-          <cell r="D63" t="str">
+          <cell r="E63" t="str">
             <v>Suspender tareas en lote hasta condicion</v>
           </cell>
         </row>
         <row r="64">
-          <cell r="D64" t="str">
+          <cell r="E64" t="str">
             <v>Actualizar comentario</v>
           </cell>
         </row>
         <row r="65">
-          <cell r="D65" t="str">
+          <cell r="E65" t="str">
             <v>Obtener información abstracta de mi tarea</v>
           </cell>
         </row>
         <row r="66">
-          <cell r="D66" t="str">
+          <cell r="E66" t="str">
             <v>Obtener información detallada de mi tarea</v>
           </cell>
         </row>
         <row r="67">
-          <cell r="D67" t="str">
+          <cell r="E67" t="str">
             <v>Consultar tareas</v>
           </cell>
         </row>
         <row r="68">
-          <cell r="D68" t="str">
+          <cell r="E68" t="str">
             <v>Activar la tarea</v>
           </cell>
         </row>
         <row r="69">
-          <cell r="D69" t="str">
+          <cell r="E69" t="str">
             <v>Activar la tarea en lote</v>
           </cell>
         </row>
         <row r="70">
-          <cell r="D70" t="str">
+          <cell r="E70" t="str">
             <v>Nominar la tarea</v>
           </cell>
         </row>
         <row r="71">
-          <cell r="D71" t="str">
+          <cell r="E71" t="str">
             <v>Nominar tareas en lote</v>
           </cell>
         </row>
         <row r="72">
-          <cell r="D72" t="str">
+          <cell r="E72" t="str">
             <v>Establecer role humano generico</v>
           </cell>
         </row>
         <row r="73">
-          <cell r="D73" t="str">
+          <cell r="E73" t="str">
             <v>Establecer roles humanos generico en lote</v>
           </cell>
         </row>
         <row r="75">
-          <cell r="D75" t="str">
+          <cell r="E75" t="str">
             <v>Registrar la definición de una tarea lean</v>
           </cell>
         </row>
         <row r="76">
-          <cell r="D76" t="str">
+          <cell r="E76" t="str">
             <v>Retirar registro de definición de tarea lean</v>
           </cell>
         </row>
         <row r="77">
-          <cell r="D77" t="str">
+          <cell r="E77" t="str">
             <v>Listar las definiciones de tareas lean</v>
           </cell>
         </row>
         <row r="78">
-          <cell r="D78" t="str">
+          <cell r="E78" t="str">
             <v>Crear una tarea lean</v>
           </cell>
         </row>
         <row r="79">
-          <cell r="D79" t="str">
+          <cell r="E79" t="str">
             <v>Crear una tarea lean asíncrona</v>
           </cell>
         </row>
@@ -1460,29 +1616,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44" style="18" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="45.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="13" style="9" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" style="18" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="9"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1492,7 +1652,7 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -1501,8 +1661,20 @@
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="G3" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1512,7 +1684,7 @@
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1521,8 +1693,18 @@
       <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="G4" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H4" s="18" t="str">
+        <f t="shared" ref="H4:H35" si="0">IFERROR(VLOOKUP(G4,ESCENARIOS_NEGOCIO,2,FALSE),"(TBD)")</f>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="C5" s="7"/>
       <c r="E5" s="8" t="s">
@@ -1531,13 +1713,18 @@
       <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -1546,13 +1733,23 @@
       <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="G6" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1561,8 +1758,18 @@
       <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1572,7 +1779,7 @@
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="18" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -1581,13 +1788,18 @@
       <c r="F8" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="C9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="18" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -1596,8 +1808,13 @@
       <c r="F9" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -1607,7 +1824,7 @@
       <c r="C10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -1616,13 +1833,20 @@
       <c r="F10" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="G10" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Registro de Definiciones de Tarea</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1631,8 +1855,13 @@
       <c r="F11" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -1642,7 +1871,7 @@
       <c r="C12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="18" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="8" t="s">
@@ -1651,8 +1880,13 @@
       <c r="F12" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
@@ -1662,925 +1896,1350 @@
       <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$3</f>
+      <c r="D13" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$3</f>
         <v>Añadir adjuntos</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="C14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$4</f>
+      <c r="D14" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$4</f>
         <v>Añadir comentario</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="C15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$5</f>
+      <c r="D15" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$5</f>
         <v>Reclamar la tarea</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="C16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$6</f>
+      <c r="D16" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$6</f>
         <v>Realizar reclamo de tarea en lote</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="C17" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$7</f>
+      <c r="D17" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$7</f>
         <v>Marcar tarea completada</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$8</f>
+      <c r="D18" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$8</f>
         <v>Marcar tarea completada en lote</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="C19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$9</f>
+      <c r="D19" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$9</f>
         <v>Delegar la tarea</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$10</f>
+      <c r="D20" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$10</f>
         <v>Delegar la tarea en lote</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="C21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$11</f>
+      <c r="D21" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$11</f>
         <v>Eliminar adjunto</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="C22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$12</f>
+      <c r="D22" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$12</f>
         <v>Eliminar comentario</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="C23" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$13</f>
+      <c r="D23" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$13</f>
         <v>Eliminar falla</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="C24" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$14</f>
+      <c r="D24" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$14</f>
         <v>Eliminar salida de la tarea</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="C25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$15</f>
+      <c r="D25" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$15</f>
         <v>Fallar la tarea</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="C26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$16</f>
+      <c r="D26" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$16</f>
         <v>Fallar tareas en lote</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="C27" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$17</f>
+      <c r="D27" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$17</f>
         <v>Mover tarea adelante</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" s="2"/>
+      <c r="H27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="C28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$18</f>
+      <c r="D28" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$18</f>
         <v>Mover tarea adelante en lote</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="C29" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$19</f>
+      <c r="D29" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$19</f>
         <v>Obtener adjunto</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" s="2"/>
+      <c r="H29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="C30" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$20</f>
+      <c r="D30" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$20</f>
         <v>Obtener información de adjuntos</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="C31" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$21</f>
+      <c r="D31" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$21</f>
         <v>Obtener comentarios</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H31" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="C32" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$22</f>
+      <c r="D32" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$22</f>
         <v>Obtener falla de tarea</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="C33" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$23</f>
+      <c r="D33" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$23</f>
         <v>Obtener información de entrada a la tarea</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H33" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="C34" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$24</f>
+      <c r="D34" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$24</f>
         <v>Obtener resultado de accion de finalización de la tarea</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="C35" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$25</f>
+      <c r="D35" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$25</f>
         <v>Obtener salida de la tarea</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="C36" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$26</f>
+      <c r="D36" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$26</f>
         <v>Obtener la tarea padre</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="str">
+        <f t="shared" ref="H36:H67" si="1">IFERROR(VLOOKUP(G36,ESCENARIOS_NEGOCIO,2,FALSE),"(TBD)")</f>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="C37" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$27</f>
+      <c r="D37" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$27</f>
         <v>Obtener Identificador de la tarea padre</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="C38" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$28</f>
+      <c r="D38" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$28</f>
         <v>Obtener visualización de la tarea</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H38" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="C39" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D39" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$29</f>
+      <c r="D39" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$29</f>
         <v>Obtener tipos de visualizaciones</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H39" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="C40" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$30</f>
+      <c r="D40" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$30</f>
         <v>Obtener identificadores de la tarea</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="C41" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$31</f>
+      <c r="D41" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$31</f>
         <v>Obtener Subtareas</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H41" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="C42" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$32</f>
+      <c r="D42" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$32</f>
         <v>Obtener Descripcion de la tarea</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H42" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="C43" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D43" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$33</f>
+      <c r="D43" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$33</f>
         <v>Obtener detalles de la tarea</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H43" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="C44" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$34</f>
+      <c r="D44" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$34</f>
         <v>Obtener historia de la tarea</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H44" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="C45" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$35</f>
+      <c r="D45" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$35</f>
         <v>Obteher Datos de Instancia de la Tarea</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H45" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="C46" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$36</f>
+      <c r="D46" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$36</f>
         <v>Obtener las operaciones de la tarea</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H46" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="C47" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$37</f>
+      <c r="D47" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$37</f>
         <v>Determinar si tiene subtareas</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G47" s="2"/>
+      <c r="H47" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="C48" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$38</f>
+      <c r="D48" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$38</f>
         <v>Instanciar subtarea</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G48" s="2"/>
+      <c r="H48" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="C49" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$39</f>
+      <c r="D49" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$39</f>
         <v>Determinar si es una subtarea</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G49" s="2"/>
+      <c r="H49" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="C50" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D50" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$40</f>
+      <c r="D50" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$40</f>
         <v>Liberar la tarea</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G50" s="2"/>
+      <c r="H50" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="C51" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D51" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$41</f>
+      <c r="D51" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$41</f>
         <v>Liberar tareas en lote</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G51" s="2"/>
+      <c r="H51" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="C52" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$42</f>
+      <c r="D52" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$42</f>
         <v>Remover tarea</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="C53" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D53" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$43</f>
-        <v>Remiver tarea en lote</v>
+      <c r="D53" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$43</f>
+        <v>Remover tarea en lote</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G53" s="2"/>
+      <c r="H53" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="C54" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D54" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$44</f>
+      <c r="D54" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$44</f>
         <v>Re-iniciar la tarea</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G54" s="2"/>
+      <c r="H54" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="C55" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D55" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$45</f>
+      <c r="D55" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$45</f>
         <v>Re-iniciar tareas en lote</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G55" s="2"/>
+      <c r="H55" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="C56" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$46</f>
+      <c r="D56" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$46</f>
         <v>Establecer falla de la tarea</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G56" s="2"/>
+      <c r="H56" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="C57" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D57" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$47</f>
+      <c r="D57" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$47</f>
         <v>Establecer la salida de la tarea</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G57" s="2"/>
+      <c r="H57" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="C58" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D58" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$48</f>
+      <c r="D58" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$48</f>
         <v>Establecer la prioridad</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G58" s="2"/>
+      <c r="H58" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="C59" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D59" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$49</f>
+      <c r="D59" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$49</f>
         <v>Establecer prioridad en lote</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G59" s="2"/>
+      <c r="H59" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="C60" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D60" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$50</f>
+      <c r="D60" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$50</f>
         <v>Establecer Expresion de fecha limite de completamiento</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G60" s="2"/>
+      <c r="H60" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="C61" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D61" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$51</f>
+      <c r="D61" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$51</f>
         <v>Establecer Expresion de fecha limite de duracion</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G61" s="2"/>
+      <c r="H61" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="C62" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D62" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$52</f>
+      <c r="D62" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$52</f>
         <v>Establecer Expresión de fecha limite para inicio de tarea</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G62" s="2"/>
+      <c r="H62" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="C63" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D63" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$53</f>
+      <c r="D63" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$53</f>
         <v>Establecer expresion de duración de inicio de tarea</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G63" s="2"/>
+      <c r="H63" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="C64" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D64" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$54</f>
+      <c r="D64" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$54</f>
         <v>Saltar la tarea</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G64" s="2"/>
+      <c r="H64" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="C65" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D65" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$55</f>
+      <c r="D65" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$55</f>
         <v>Saltar tareas en lote</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G65" s="2"/>
+      <c r="H65" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="C66" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D66" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$56</f>
+      <c r="D66" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$56</f>
         <v>Iniciar la tarea</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G66" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H66" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="C67" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D67" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$57</f>
+      <c r="D67" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$57</f>
         <v>Iniciar tareas en lote</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G67" s="2"/>
+      <c r="H67" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="C68" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D68" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$58</f>
+      <c r="D68" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$58</f>
         <v>Detener tarea</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G68" s="2"/>
+      <c r="H68" s="2" t="str">
+        <f t="shared" ref="H68:H90" si="2">IFERROR(VLOOKUP(G68,ESCENARIOS_NEGOCIO,2,FALSE),"(TBD)")</f>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="C69" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D69" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$59</f>
+      <c r="D69" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$59</f>
         <v>Detener tareas en lote</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G69" s="2"/>
+      <c r="H69" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="C70" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D70" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$60</f>
+      <c r="D70" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$60</f>
         <v>Suspender la tarea</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G70" s="2"/>
+      <c r="H70" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="C71" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D71" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$61</f>
+      <c r="D71" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$61</f>
         <v>Suspender tareas en lote</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G71" s="2"/>
+      <c r="H71" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="C72" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D72" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$62</f>
+      <c r="D72" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$62</f>
         <v>Suspender tarea hasta condicion</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G72" s="2"/>
+      <c r="H72" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="C73" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D73" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$63</f>
+      <c r="D73" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$63</f>
         <v>Suspender tareas en lote hasta condicion</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G73" s="2"/>
+      <c r="H73" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="C74" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D74" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$64</f>
+      <c r="D74" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$64</f>
         <v>Actualizar comentario</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G74" s="2"/>
+      <c r="H74" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="C75" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D75" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$65</f>
+      <c r="D75" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$65</f>
         <v>Obtener información abstracta de mi tarea</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G75" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H75" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="C76" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D76" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$66</f>
+      <c r="D76" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$66</f>
         <v>Obtener información detallada de mi tarea</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G76" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H76" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="C77" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D77" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$67</f>
+      <c r="D77" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$67</f>
         <v>Consultar tareas</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G77" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H77" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>Ejecución de una tarea de negocio</v>
+      </c>
+      <c r="I77" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="C78" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D78" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$68</f>
+      <c r="D78" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$68</f>
         <v>Activar la tarea</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G78" s="2"/>
+      <c r="H78" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="C79" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D79" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$69</f>
+      <c r="D79" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$69</f>
         <v>Activar la tarea en lote</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G79" s="2"/>
+      <c r="H79" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="C80" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D80" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$70</f>
+      <c r="D80" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$70</f>
         <v>Nominar la tarea</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G80" s="2"/>
+      <c r="H80" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="C81" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D81" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$71</f>
+      <c r="D81" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$71</f>
         <v>Nominar tareas en lote</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G81" s="2"/>
+      <c r="H81" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="C82" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D82" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$72</f>
+      <c r="D82" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$72</f>
         <v>Establecer role humano generico</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G82" s="2"/>
+      <c r="H82" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="C83" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D83" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$73</f>
+      <c r="D83" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$73</f>
         <v>Establecer roles humanos generico en lote</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G83" s="2"/>
+      <c r="H83" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>49</v>
       </c>
@@ -2590,67 +3249,92 @@
       <c r="C84" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D84" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$75</f>
+      <c r="D84" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$75</f>
         <v>Registrar la definición de una tarea lean</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G84" s="2"/>
+      <c r="H84" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="C85" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D85" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$76</f>
+      <c r="D85" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$76</f>
         <v>Retirar registro de definición de tarea lean</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G85" s="2"/>
+      <c r="H85" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="C86" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D86" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$77</f>
+      <c r="D86" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$77</f>
         <v>Listar las definiciones de tareas lean</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G86" s="2"/>
+      <c r="H86" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="C87" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D87" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$78</f>
+      <c r="D87" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$78</f>
         <v>Crear una tarea lean</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G87" s="2"/>
+      <c r="H87" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="C88" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D88" s="2" t="str">
-        <f>[1]PORTAFOLIO_SERVICIOS!$D$79</f>
+      <c r="D88" s="18" t="str">
+        <f>[1]PORTAFOLIO_SERVICIOS!$E$79</f>
         <v>Crear una tarea lean asíncrona</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G88" s="2"/>
+      <c r="H88" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>51</v>
       </c>
@@ -2658,11 +3342,16 @@
         <v>47</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>54</v>
+        <v>207</v>
       </c>
       <c r="E89" s="8"/>
-    </row>
-    <row r="90" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G89" s="2"/>
+      <c r="H89" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>52</v>
       </c>
@@ -2672,13 +3361,188 @@
       <c r="C90" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D90" s="18" t="s">
         <v>130</v>
       </c>
       <c r="E90" s="8"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>(TBD)</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:J90">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="EN001"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" style="11" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="16"/>
+    <col min="3" max="3" width="47.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="88" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Definicion de User Story US009.01 Perfil del Usuario
</commit_message>
<xml_diff>
--- a/Requerimientos/Backlog_producto.xlsx
+++ b/Requerimientos/Backlog_producto.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FEATURES!$A$3:$J$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FEATURES!$A$3:$J$95</definedName>
     <definedName name="ESCENARIOS_NEGOCIO">ESCENARIOS_NEGOCIO!$B$3:$E$19</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="247">
   <si>
     <t>BACKLOG DEL PRODUCTO</t>
   </si>
@@ -712,6 +712,67 @@
   </si>
   <si>
     <t>SP2</t>
+  </si>
+  <si>
+    <t>EN004</t>
+  </si>
+  <si>
+    <t>Actualización de Perfil del Usuario</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresa a la información de su perfil.
+2. El usuario cambia preferencia de idioma
+3. El usuario cambia su información personal del directorio de gestión de identidades (Nick name, Foto)
+4. El usuario registra los cambios a su perfil.
+5. El worklist cambia la configuración de idioma de acuerdo con la preferencia establecida.</t>
+  </si>
+  <si>
+    <t>FEAT-009</t>
+  </si>
+  <si>
+    <t>Personalización del perfil del usuario</t>
+  </si>
+  <si>
+    <t>US-009.01</t>
+  </si>
+  <si>
+    <t>Cambio de idioma</t>
+  </si>
+  <si>
+    <t>US-009.02</t>
+  </si>
+  <si>
+    <t>Cambio de información personal</t>
+  </si>
+  <si>
+    <t>CA-009.01.01</t>
+  </si>
+  <si>
+    <t>El usuario realiza el cambio de su idioma y el worklist desde ese momento presnta la información conforme al idioma seleccionado.</t>
+  </si>
+  <si>
+    <t>El usuario realiza el cambio de su idioma y el worklist desde ese momento presnta la información conforme al idioma seleccionado y al no existir una traducción para el idioma seleccionado se utilizará el idioma por defecto del worklist.</t>
+  </si>
+  <si>
+    <t>CA-009.01.02</t>
+  </si>
+  <si>
+    <t>CA-009.02.01</t>
+  </si>
+  <si>
+    <t>El usuario cambia su nickname y este aparece en la página principal del Worklist</t>
+  </si>
+  <si>
+    <t>CA-009.02.02</t>
+  </si>
+  <si>
+    <t>El usuario cambia su foto y esta aparece junto al nickname en la página principal del worklist.</t>
+  </si>
+  <si>
+    <t>El usuario cambia su foto y esta aparece junto al nickname en los comentarios asociados a las tareas.</t>
   </si>
 </sst>
 </file>
@@ -848,7 +909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -918,6 +979,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1623,10 +1687,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1636,7 +1700,7 @@
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
     <col min="4" max="4" width="44" style="18" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="45.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="74.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="13" style="9" customWidth="1"/>
     <col min="8" max="8" width="36.7109375" style="18" customWidth="1"/>
     <col min="9" max="10" width="9.140625" style="9"/>
@@ -2998,7 +3062,7 @@
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2" t="str">
-        <f t="shared" ref="H68:H90" si="2">IFERROR(VLOOKUP(G68,ESCENARIOS_NEGOCIO,2,FALSE),"(TBD)")</f>
+        <f t="shared" ref="H68:H94" si="2">IFERROR(VLOOKUP(G68,ESCENARIOS_NEGOCIO,2,FALSE),"(TBD)")</f>
         <v>(TBD)</v>
       </c>
     </row>
@@ -3242,7 +3306,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="C81" s="7" t="s">
         <v>122</v>
@@ -3260,7 +3324,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="C82" s="7" t="s">
         <v>123</v>
@@ -3278,7 +3342,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="C83" s="7" t="s">
         <v>124</v>
@@ -3296,7 +3360,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>49</v>
       </c>
@@ -3319,7 +3383,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="C85" s="7" t="s">
         <v>125</v>
@@ -3337,7 +3401,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="C86" s="7" t="s">
         <v>126</v>
@@ -3355,7 +3419,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="C87" s="7" t="s">
         <v>127</v>
@@ -3373,7 +3437,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="C88" s="7" t="s">
         <v>128</v>
@@ -3391,7 +3455,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>51</v>
       </c>
@@ -3408,7 +3472,7 @@
         <v>(TBD)</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>52</v>
       </c>
@@ -3428,12 +3492,143 @@
         <v>(TBD)</v>
       </c>
     </row>
+    <row r="91" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H91" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Actualización de Perfil del Usuario</v>
+      </c>
+      <c r="I91" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J91" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A92" s="6"/>
+      <c r="C92" s="7"/>
+      <c r="E92" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H92" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Actualización de Perfil del Usuario</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J92" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="6"/>
+      <c r="C93" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H93" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Actualización de Perfil del Usuario</v>
+      </c>
+      <c r="I93" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J93" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="6"/>
+      <c r="C94" s="7"/>
+      <c r="E94" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H94" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Actualización de Perfil del Usuario</v>
+      </c>
+      <c r="I94" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J94" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A95" s="6"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H95" s="2" t="str">
+        <f t="shared" ref="H95" si="3">IFERROR(VLOOKUP(G95,ESCENARIOS_NEGOCIO,2,FALSE),"(TBD)")</f>
+        <v>Actualización de Perfil del Usuario</v>
+      </c>
+      <c r="I95" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J95" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A3:J90">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="EN001"/>
-      </filters>
+  <autoFilter ref="A3:J95">
+    <filterColumn colId="8">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
     <filterColumn colId="9">
       <filters>
@@ -3450,8 +3645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3520,11 +3715,19 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="15"/>
+    <row r="6" spans="2:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>

</xml_diff>